<commit_message>
Cubo roda traseira lander
</commit_message>
<xml_diff>
--- a/moto2020.xlsx
+++ b/moto2020.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="44">
   <si>
     <t>km</t>
   </si>
@@ -140,6 +140,21 @@
   </si>
   <si>
     <t>Total dia</t>
+  </si>
+  <si>
+    <t>cubo tras</t>
+  </si>
+  <si>
+    <t>raios traseiros</t>
+  </si>
+  <si>
+    <t>troca</t>
+  </si>
+  <si>
+    <t>rolamentos roda tras</t>
+  </si>
+  <si>
+    <t>pastilha freio diant</t>
   </si>
 </sst>
 </file>
@@ -571,7 +586,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -671,6 +686,8 @@
     </xf>
     <xf numFmtId="16" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6443,7 +6460,7 @@
   <dimension ref="A2:U105"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -8096,83 +8113,146 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:J100"/>
+  <dimension ref="A2:O96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="8.7109375" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" customWidth="1"/>
-    <col min="4" max="4" width="7.5703125" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" customWidth="1"/>
-    <col min="9" max="9" width="7.28515625" customWidth="1"/>
-    <col min="10" max="11" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" customWidth="1"/>
+    <col min="6" max="6" width="7.5703125" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" customWidth="1"/>
+    <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" customWidth="1"/>
+    <col min="11" max="11" width="7.28515625" customWidth="1"/>
+    <col min="12" max="13" width="8.7109375" customWidth="1"/>
+    <col min="15" max="15" width="19.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="51" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="52" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="51" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I2" t="s">
         <v>12</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>13</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>14</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="H3">
+      <c r="M2" t="s">
+        <v>39</v>
+      </c>
+      <c r="N2" t="s">
+        <v>40</v>
+      </c>
+      <c r="O2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C3">
         <v>63764</v>
       </c>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="G4">
+      <c r="J3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C4">
         <v>79581</v>
       </c>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="H5">
+      <c r="I4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C5">
         <v>81021</v>
       </c>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="H9">
-        <f>H5-H3</f>
-        <v>17257</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D10">
+      <c r="J5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C6">
         <v>118361</v>
       </c>
-      <c r="E10">
-        <v>118361</v>
-      </c>
-    </row>
+      <c r="F6" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="61">
+        <v>43898</v>
+      </c>
+      <c r="B7">
+        <v>440</v>
+      </c>
+      <c r="C7">
+        <v>124301</v>
+      </c>
+      <c r="D7">
+        <v>36</v>
+      </c>
+      <c r="E7">
+        <v>20</v>
+      </c>
+      <c r="H7">
+        <v>30</v>
+      </c>
+      <c r="M7">
+        <v>170</v>
+      </c>
+      <c r="N7">
+        <v>70</v>
+      </c>
+      <c r="O7">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H15" s="62"/>
+      <c r="I15" s="62"/>
+    </row>
+    <row r="17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -8249,12 +8329,8 @@
     <row r="94" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="95" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="96" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="97" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="98" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="99" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="100" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>